<commit_message>
add radio test software with CLI; station selection now done in config file as an index; spreadsheet for TX power calcs.
</commit_message>
<xml_diff>
--- a/Docs/misc/power_levels.xlsx
+++ b/Docs/misc/power_levels.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22340" yWindow="6920" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="3460" yWindow="3900" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ALC Voltage sensitvity" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Watts</t>
   </si>
@@ -27,14 +28,79 @@
     <t>dBm</t>
   </si>
   <si>
-    <t>dBm Delta</t>
+    <t>dB Delta</t>
+  </si>
+  <si>
+    <t>R1 = - Vout/10uA</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t>E192 Closeest value</t>
+  </si>
+  <si>
+    <t>next lower</t>
+  </si>
+  <si>
+    <t>next higher</t>
+  </si>
+  <si>
+    <t>+1%</t>
+  </si>
+  <si>
+    <t>-1%</t>
+  </si>
+  <si>
+    <t>+.1%</t>
+  </si>
+  <si>
+    <t>-.1%</t>
+  </si>
+  <si>
+    <t>% Err</t>
+  </si>
+  <si>
+    <t>5ppm/C</t>
+  </si>
+  <si>
+    <t>5ppm/°C</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>25ppm/C</t>
+  </si>
+  <si>
+    <t>50ppm/C</t>
+  </si>
+  <si>
+    <t>100ppm/C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,39 +149,93 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="23" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="23" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="50">
+    <cellStyle name="Comma" xfId="23" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -127,6 +247,19 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -138,6 +271,19 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D16"/>
+  <dimension ref="B1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -507,6 +653,10 @@
         <f t="shared" ref="C3:C5" si="0">10*LOG10(B3/0.001)</f>
         <v>40</v>
       </c>
+      <c r="D3">
+        <f>C2-C3</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4">
@@ -516,6 +666,10 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D5" si="1">C3-C4</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5">
@@ -524,6 +678,10 @@
       <c r="C5">
         <f t="shared" si="0"/>
         <v>20</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -537,7 +695,7 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="1">
-        <f t="shared" ref="B8:B10" si="1">POWER(10,C8/10)/1000</f>
+        <f t="shared" ref="B8:B10" si="2">POWER(10,C8/10)/1000</f>
         <v>10</v>
       </c>
       <c r="C8">
@@ -550,33 +708,33 @@
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.511886431509581</v>
       </c>
       <c r="C9">
         <v>34</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D10" si="2">C8-C9</f>
+        <f t="shared" ref="D9:D10" si="3">C8-C9</f>
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.63095734448019325</v>
       </c>
       <c r="C10">
         <v>28</v>
       </c>
       <c r="D10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="1">
-        <f t="shared" ref="B13:B15" si="3">POWER(10,C13/10)/1000</f>
+        <f t="shared" ref="B13:B15" si="4">POWER(10,C13/10)/1000</f>
         <v>95.000000000000057</v>
       </c>
       <c r="C13">
@@ -589,7 +747,7 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.056485328380596</v>
       </c>
       <c r="C14">
@@ -602,7 +760,7 @@
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.7820181202582228</v>
       </c>
       <c r="C15">
@@ -618,9 +776,60 @@
         <v>0.95</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16" si="4">10*LOG10(B16/0.001)</f>
+        <f t="shared" ref="C16" si="5">10*LOG10(B16/0.001)</f>
         <v>29.777236052888476</v>
       </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18">
+        <f>10*LOG10(B18/0.001)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:C21" si="6">10*LOG10(B19/0.001)</f>
+        <v>40</v>
+      </c>
+      <c r="D19">
+        <f>C18-C19</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20">
+        <v>1.2</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="6"/>
+        <v>30.791812460476248</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:D21" si="7">C19-C20</f>
+        <v>9.2081875395237525</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21">
+        <v>0.1</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="7"/>
+        <v>10.791812460476248</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -631,4 +840,327 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>0.96</v>
+      </c>
+      <c r="B7" s="3">
+        <f>A7/0.00001</f>
+        <v>95999.999999999985</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" ref="B8:B10" si="0">A8/0.00001</f>
+        <v>2200000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>-8</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>-799999.99999999988</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>0.96</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>95999.999999999985</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" ht="18">
+      <c r="B12" s="3"/>
+      <c r="H12" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="45" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="E13" s="11">
+        <v>1E-3</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="B14" s="4"/>
+      <c r="H14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="14">
+        <v>25</v>
+      </c>
+      <c r="J14" s="14">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>96000</v>
+      </c>
+      <c r="B15" s="4">
+        <f>A15*0.00001</f>
+        <v>0.96000000000000008</v>
+      </c>
+      <c r="H15" s="15">
+        <f>($H$14-$I$14)*0.000005</f>
+        <v>-1.25E-4</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" s="16">
+        <f>($J$14-$I$14)*0.000005</f>
+        <v>3.0000000000000003E-4</v>
+      </c>
+      <c r="K15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>96500</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" ref="B16:B22" si="1">A16*0.00001</f>
+        <v>0.96500000000000008</v>
+      </c>
+      <c r="C16" s="5">
+        <f>($B$15-B16)/$B$15</f>
+        <v>-5.2083333333333374E-3</v>
+      </c>
+      <c r="D16">
+        <f>A16*0.01</f>
+        <v>965</v>
+      </c>
+      <c r="E16">
+        <f>A16*0.001</f>
+        <v>96.5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="15">
+        <f>($H$14-$I$14)*0.000025</f>
+        <v>-6.2500000000000001E-4</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="16">
+        <f>($J$14-$I$14)*0.000025</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="K16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>95300</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" si="1"/>
+        <v>0.95300000000000007</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" ref="C17:C22" si="2">($B$15-B17)/$B$15</f>
+        <v>7.2916666666666729E-3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="15">
+        <f>($H$14-$I$14)*0.00005</f>
+        <v>-1.25E-3</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="16">
+        <f>($J$14-$I$14)*0.00005</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>97600</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="1"/>
+        <v>0.97600000000000009</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.666666666666668E-2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="15">
+        <f>($H$14-$I$14)*0.0001</f>
+        <v>-2.5000000000000001E-3</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" s="16">
+        <f>($J$14-$I$14)*0.0001</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <f>A16+D16</f>
+        <v>97465</v>
+      </c>
+      <c r="B19" s="4">
+        <f t="shared" si="1"/>
+        <v>0.97465000000000013</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.5260416666666719E-2</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <f>A16-D16</f>
+        <v>95535</v>
+      </c>
+      <c r="B20" s="4">
+        <f t="shared" si="1"/>
+        <v>0.95535000000000003</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" si="2"/>
+        <v>4.8437500000000442E-3</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <f>A16+E16</f>
+        <v>96596.5</v>
+      </c>
+      <c r="B21" s="4">
+        <f t="shared" si="1"/>
+        <v>0.96596500000000007</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" si="2"/>
+        <v>-6.2135416666666641E-3</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <f>A16-E16</f>
+        <v>96403.5</v>
+      </c>
+      <c r="B22" s="4">
+        <f t="shared" si="1"/>
+        <v>0.96403500000000009</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" si="2"/>
+        <v>-4.2031250000000107E-3</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="H26" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
testing Rev C PCBA
</commit_message>
<xml_diff>
--- a/Docs/misc/power_levels.xlsx
+++ b/Docs/misc/power_levels.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="3900" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Watts</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>100ppm/C</t>
+  </si>
+  <si>
+    <t>Above is per ohm..need to multiple by the total ohms</t>
   </si>
 </sst>
 </file>
@@ -90,8 +93,8 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0000000000"/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
-    <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -212,9 +215,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="23" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -231,8 +231,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="Comma" xfId="23" builtinId="3"/>
@@ -846,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -858,21 +861,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
@@ -923,7 +926,7 @@
     </row>
     <row r="12" spans="1:11" ht="18">
       <c r="B12" s="3"/>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -931,31 +934,31 @@
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>0.01</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>1E-3</v>
       </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:11">
       <c r="B14" s="4"/>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="13">
         <v>25</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="13">
         <v>85</v>
       </c>
     </row>
@@ -967,15 +970,15 @@
         <f>A15*0.00001</f>
         <v>0.96000000000000008</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <f>($H$14-$I$14)*0.000005</f>
         <v>-1.25E-4</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15" s="16">
-        <f>($J$14-$I$14)*0.000005</f>
+      <c r="J15" s="15">
+        <f>(($J$14-$I$14)*0.000005)</f>
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="K15" t="s">
@@ -1005,14 +1008,14 @@
       <c r="F16" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="14">
         <f>($H$14-$I$14)*0.000025</f>
         <v>-6.2500000000000001E-4</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16" s="16">
+      <c r="J16" s="15">
         <f>($J$14-$I$14)*0.000025</f>
         <v>1.5E-3</v>
       </c>
@@ -1035,14 +1038,14 @@
       <c r="F17" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="14">
         <f>($H$14-$I$14)*0.00005</f>
         <v>-1.25E-3</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
-      <c r="J17" s="16">
+      <c r="J17" s="15">
         <f>($J$14-$I$14)*0.00005</f>
         <v>3.0000000000000001E-3</v>
       </c>
@@ -1065,14 +1068,14 @@
       <c r="F18" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="14">
         <f>($H$14-$I$14)*0.0001</f>
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
-      <c r="J18" s="16">
+      <c r="J18" s="15">
         <f>($J$14-$I$14)*0.0001</f>
         <v>6.0000000000000001E-3</v>
       </c>
@@ -1113,6 +1116,9 @@
       <c r="F20" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21">
@@ -1149,7 +1155,7 @@
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="H26" s="13"/>
+      <c r="H26" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>